<commit_message>
repair SOC by violation
</commit_message>
<xml_diff>
--- a/docs/Feasibility_EVs.xlsx
+++ b/docs/Feasibility_EVs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\Charge_Pyomo\greedy\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60472AD7-31B8-4E21-9A00-422CF1EAD5A2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4534E1-FA44-402D-82DF-5EC71E93A48C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,10 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Greedy</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Y</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,6 +132,26 @@
   </si>
   <si>
     <t>100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N(failure)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Greedy(rndstop!)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>minhstop!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -185,8 +201,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,45 +498,49 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
     <col min="2" max="10" width="15.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="3"/>
     <col min="12" max="13" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -538,7 +561,7 @@
         <v>2</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M2" s="1">
         <v>113</v>
@@ -555,7 +578,7 @@
         <v>2.9759998321533199</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="1">
         <v>2371887.4716866598</v>
@@ -564,7 +587,7 @@
         <v>44.973000049591001</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="1">
         <v>39565.8411908946</v>
@@ -573,10 +596,10 @@
         <v>1.9999980926513599E-2</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M3" s="1">
         <v>96</v>
@@ -584,7 +607,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="B4" s="3">
+        <v>17925.951999409699</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.70399999618530196</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E4" s="1">
         <v>17926.267450612599</v>
@@ -593,7 +625,7 @@
         <v>4.94700002670288</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H4" s="1">
         <v>17934.747721178301</v>
@@ -602,10 +634,10 @@
         <v>0.24900007247924799</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M4" s="1">
         <v>6000</v>
@@ -613,7 +645,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="B5" s="3">
+        <v>34961.306080587899</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.8499999046325599</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E5" s="1">
         <v>34972.366492705201</v>
@@ -622,7 +663,7 @@
         <v>37.430000066757202</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="1">
         <v>34964.304114709499</v>
@@ -631,10 +672,10 @@
         <v>0.27699995040893499</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M5" s="1">
         <v>0.08</v>
@@ -642,13 +683,19 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.0909998416900599</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="F6" s="1">
         <v>37.189999818801802</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="1">
         <v>30091.663320635002</v>
@@ -657,18 +704,24 @@
         <v>0.25699996948242099</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.93099999427795399</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="F7" s="1">
         <v>19.313000202178898</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H7" s="1">
         <v>26073.003870951699</v>
@@ -677,12 +730,12 @@
         <v>0.28999996185302701</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2">
         <v>22573.3820582105</v>
@@ -691,7 +744,7 @@
         <v>148.272000074386</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2">
         <v>22415.541212552602</v>
@@ -700,14 +753,22 @@
         <v>0.35699987411499001</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B9" s="3">
+        <v>14352.025028387099</v>
+      </c>
+      <c r="C9" s="3">
+        <v>221.169999837875</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="E9" s="2">
         <v>14365.135899597801</v>
       </c>
@@ -715,7 +776,7 @@
         <v>2.5749998092651301</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" s="2">
         <v>14385.4158111862</v>
@@ -724,12 +785,21 @@
         <v>0.27800011634826599</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10658.8759252645</v>
+      </c>
+      <c r="C10" s="3">
+        <v>24.8560001850128</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E10" s="2">
         <v>10663.6341785721</v>
@@ -738,7 +808,7 @@
         <v>127.93400001525799</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" s="2">
         <v>10662.1317246201</v>
@@ -747,12 +817,24 @@
         <v>0.25499987602233798</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="3">
+        <v>7100.5354779756899</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.23100018501281699</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="E11" s="2">
         <v>7100.6637228233503</v>
@@ -761,7 +843,7 @@
         <v>1.42799997329711</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="2">
         <v>7104.7233618518003</v>
@@ -770,21 +852,30 @@
         <v>0.23699998855590801</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3607.85144045987</v>
+      </c>
+      <c r="C12" s="3">
+        <v>12.317999839782701</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="2">
-        <v>3610.4524037302399</v>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="F12" s="2">
         <v>42.144999980926499</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" s="2">
         <v>3622.0349754617901</v>
@@ -793,7 +884,7 @@
         <v>0.23799991607665999</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>